<commit_message>
Update outputs for 2024
</commit_message>
<xml_diff>
--- a/2024/RuntimesChart.xlsx
+++ b/2024/RuntimesChart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\exercises\adventOfCode\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33D5B52E-66CA-4FFB-B8B8-5A59AE0E096F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C71AEA-8668-4958-A4EA-2A52C1A76A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="1845" windowWidth="22980" windowHeight="12300" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
@@ -191,6 +191,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -200,6 +212,18 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>2.4184599999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.9999399999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2885200000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.62774E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1318,10 +1342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="A3:B20"/>
+      <selection activeCell="A3" sqref="A3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,6 +1367,38 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2.4184599999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4.9999399999999996E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2.2885200000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>4.62774E-3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Solve 2024, day 8
</commit_message>
<xml_diff>
--- a/2024/RuntimesChart.xlsx
+++ b/2024/RuntimesChart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\exercises\adventOfCode\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C71AEA-8668-4958-A4EA-2A52C1A76A8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16AA09B-3AE3-4256-9866-63CC43FBCF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1845" windowWidth="22980" windowHeight="12300" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
+    <workbookView xWindow="2370" yWindow="1410" windowWidth="22980" windowHeight="12300" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
   <sheets>
     <sheet name="RuntimesChart" sheetId="1" r:id="rId1"/>
@@ -203,6 +203,18 @@
                 <c:pt idx="3">
                   <c:v>4</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -213,16 +225,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2.4184599999999999E-3</c:v>
+                  <c:v>2.3924599999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9999399999999996E-3</c:v>
+                  <c:v>3.4427400000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2885200000000001E-3</c:v>
+                  <c:v>2.2166E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.62774E-3</c:v>
+                  <c:v>4.3159599999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.2547800000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>16.177439159999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1248556199999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.3554600000000002E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1342,10 +1366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B6"/>
+      <selection activeCell="A3" sqref="A3:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,7 +1396,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2.4184599999999999E-3</v>
+        <v>2.3924599999999999E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1380,7 +1404,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.9999399999999996E-3</v>
+        <v>3.4427400000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1388,7 +1412,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2.2885200000000001E-3</v>
+        <v>2.2166E-3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1396,7 +1420,39 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4.62774E-3</v>
+        <v>4.3159599999999998E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>9.2547800000000006E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>16.177439159999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2.1248556199999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>3.3554600000000002E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Solve 2024, day 12, part 2
</commit_message>
<xml_diff>
--- a/2024/RuntimesChart.xlsx
+++ b/2024/RuntimesChart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\exercises\adventOfCode\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16AA09B-3AE3-4256-9866-63CC43FBCF86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15983EA6-DA4E-4A3F-B6B1-E8F4AC2DAC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2370" yWindow="1410" windowWidth="22980" windowHeight="12300" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
+    <workbookView xWindow="-23016" yWindow="984" windowWidth="22992" windowHeight="12312" xr2:uid="{785DA146-5632-4A51-A7D0-71CFF5792146}"/>
   </bookViews>
   <sheets>
     <sheet name="RuntimesChart" sheetId="1" r:id="rId1"/>
@@ -215,6 +215,18 @@
                 <c:pt idx="7">
                   <c:v>8</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -225,28 +237,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>2.3924599999999999E-3</c:v>
+                  <c:v>2.7379599999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.4427400000000001E-3</c:v>
+                  <c:v>3.57888E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2166E-3</c:v>
+                  <c:v>2.00994E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.3159599999999998E-3</c:v>
+                  <c:v>4.3233999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2547800000000006E-3</c:v>
+                  <c:v>1.0369079999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16.177439159999999</c:v>
+                  <c:v>15.880498640000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.1248556199999999</c:v>
+                  <c:v>2.1064885200000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.3554600000000002E-3</c:v>
+                  <c:v>3.09516E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.14254684000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5152519999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.0809299999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.4846819999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1366,10 +1390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F92283-75AE-4EA8-BD8D-63ABCF1CEF1C}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B10"/>
+      <selection activeCell="A3" sqref="A3:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,7 +1420,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2.3924599999999999E-3</v>
+        <v>2.7379599999999998E-3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1404,7 +1428,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>3.4427400000000001E-3</v>
+        <v>3.57888E-3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1412,7 +1436,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2.2166E-3</v>
+        <v>2.00994E-3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1420,7 +1444,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>4.3159599999999998E-3</v>
+        <v>4.3233999999999998E-3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1428,7 +1452,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>9.2547800000000006E-3</v>
+        <v>1.0369079999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1436,7 +1460,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>16.177439159999999</v>
+        <v>15.880498640000001</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1444,7 +1468,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2.1248556199999999</v>
+        <v>2.1064885200000001</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1452,7 +1476,39 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3.3554600000000002E-3</v>
+        <v>3.09516E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.14254684000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1.5152519999999999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>9.0809299999999996E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>6.4846819999999999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>